<commit_message>
rounding up account value
</commit_message>
<xml_diff>
--- a/RWA1 - Casos de Teste_Bug Report_Test Report.xlsx
+++ b/RWA1 - Casos de Teste_Bug Report_Test Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biage\Development\lume\cypress-realworld-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F3B31F9-CA69-4040-943E-9AF8A85006E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF62155-3F2F-44F6-8927-E25A1D5D6BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="773" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="120">
   <si>
     <t>Passos</t>
   </si>
@@ -173,30 +173,9 @@
     <t>Data</t>
   </si>
   <si>
-    <t>Aparecer o valor subtotal com duas casas decimais após o ponto</t>
-  </si>
-  <si>
-    <t>Está aparecendo um valor com diversas casas decimais após o ponto</t>
-  </si>
-  <si>
     <t>Produção</t>
   </si>
   <si>
-    <t>Médio</t>
-  </si>
-  <si>
-    <t>Checkout Overview -&gt; Subtotal possui muitas casas decimais após o ponto</t>
-  </si>
-  <si>
-    <t>Checkout: Your Information -&gt; Campo Zip/Postal Code aceita letras</t>
-  </si>
-  <si>
-    <t>No campo Zip/Postal Code aceitar apenas números</t>
-  </si>
-  <si>
-    <t>Campo Zip/Postal Code aceita letras e outros caracteres</t>
-  </si>
-  <si>
     <t>Caso de Teste</t>
   </si>
   <si>
@@ -212,17 +191,6 @@
     <t># Bug Report</t>
   </si>
   <si>
-    <t>1. Selecionar diversos produtos para o carrinho
-2. Clique em Checkout
-3. Preencher informações do usuário</t>
-  </si>
-  <si>
-    <t>1. Selecionar diversos produtos para o carrinho
-2. Clique em Checkout
-3. Preencher informações do usuário
-4. Ir para a página de Checkout Overview</t>
-  </si>
-  <si>
     <t>Ver aba Evidência Bug Report</t>
   </si>
   <si>
@@ -253,12 +221,6 @@
     <t>Feature</t>
   </si>
   <si>
-    <t>4.4.3</t>
-  </si>
-  <si>
-    <t>5.1.2</t>
-  </si>
-  <si>
     <t>Resultados Esperados</t>
   </si>
   <si>
@@ -269,9 +231,6 @@
   </si>
   <si>
     <t>Bug Report #1</t>
-  </si>
-  <si>
-    <t>Bug Report #2</t>
   </si>
   <si>
     <t>Referência Bug Report</t>
@@ -404,13 +363,52 @@
     <t>3.2.1</t>
   </si>
   <si>
-    <t>Garanta que o sistema exiba uma mensagem de erro ao tentar enviar dinheiro sem saldo suficiente.</t>
-  </si>
-  <si>
     <t>Deve enviar dinheiro com sucesso</t>
   </si>
   <si>
-    <t>Deve exibir mensagem de erro ao enviar dinheiro sem saldo suficiente</t>
+    <t>Acessar página de Transação do sistema</t>
+  </si>
+  <si>
+    <t>Digite o nome do contato</t>
+  </si>
+  <si>
+    <t>Digite o valor da transferência igual ou menor que o saldo bancário</t>
+  </si>
+  <si>
+    <t>Clique no botão "Pay"</t>
+  </si>
+  <si>
+    <t>3.1.2</t>
+  </si>
+  <si>
+    <t>3.1.3</t>
+  </si>
+  <si>
+    <t>Digite o valor da transferência maior que o saldo bancário</t>
+  </si>
+  <si>
+    <t>O botão "Pay" deve estar desabilitado para que não seja possível prosseguir com a transação.</t>
+  </si>
+  <si>
+    <t>Verificar se o botão "Pay" está desabilitado</t>
+  </si>
+  <si>
+    <t>3.2.2</t>
+  </si>
+  <si>
+    <t>3.2.3</t>
+  </si>
+  <si>
+    <t>Botão "Pay" está habilitado para prosseguir com a operação</t>
+  </si>
+  <si>
+    <t>Botão "Pay" habilitado para transação com saldo insuficiente</t>
+  </si>
+  <si>
+    <t>1. Acessar página de Transação do sistema
+2. Digite o nome do contato
+3. Digite o valor da transferência maior que o saldo bancário
+4. Verificar se o botão "Pay" está desabilitado</t>
   </si>
 </sst>
 </file>
@@ -570,7 +568,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -591,19 +589,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -677,24 +662,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -721,7 +693,7 @@
     <xf numFmtId="1" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -750,9 +722,6 @@
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -787,38 +756,32 @@
     <xf numFmtId="1" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -827,9 +790,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="9" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="9" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -841,10 +801,31 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -882,23 +863,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>43542</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>43543</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>4026106</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>2355970</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>4780641</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>2372141</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagem 1">
+        <xdr:cNvPr id="4" name="Imagem 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30EB922F-874B-47EE-A55A-AE9D330E523B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{037A3A67-CB53-D325-EEBA-83561EFE3978}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -914,52 +895,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1466850" y="2108200"/>
-          <a:ext cx="4007056" cy="2330570"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>374650</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>2946400</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>2406650</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagem 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10C36BBB-F106-427D-99FD-8DA41E43D0C8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5981700" y="2635249"/>
-          <a:ext cx="2571750" cy="2330451"/>
+          <a:off x="2102756" y="2628900"/>
+          <a:ext cx="4737099" cy="2328598"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -976,22 +913,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>215900</xdr:colOff>
+      <xdr:colOff>12700</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>4222956</xdr:colOff>
+      <xdr:colOff>4749799</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>2482970</xdr:rowOff>
+      <xdr:rowOff>2366698</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagem 1">
+        <xdr:cNvPr id="4" name="Imagem 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B06CFA4-1540-49BE-9018-C0D6335ABA1B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F26C338B-2D20-444E-B403-419FF25ED299}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1007,52 +944,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="825500" y="482600"/>
-          <a:ext cx="4007056" cy="2330570"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1041400</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>3613150</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>2529543</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagem 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98465016-F971-4521-BC0E-18CDBC1431ED}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1651000" y="2667000"/>
-          <a:ext cx="2571750" cy="2485093"/>
+          <a:off x="965200" y="412750"/>
+          <a:ext cx="4737099" cy="2328598"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1265,11 +1158,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1303,22 +1196,22 @@
     </row>
     <row r="2" spans="1:11" s="15" customFormat="1" ht="26" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="G2" s="13" t="s">
         <v>2</v>
@@ -1326,87 +1219,87 @@
       <c r="H2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="33" t="s">
-        <v>71</v>
+      <c r="K2" s="32" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="F3" s="12"/>
       <c r="G3" s="19" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="H3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="K3" s="35">
+      <c r="J3" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="K3" s="34">
         <f>SUM(K4:K7)</f>
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="17" customFormat="1" ht="13" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="19" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="H4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="36" t="s">
+      <c r="J4" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="K4" s="37">
+      <c r="K4" s="36">
         <f>COUNTIF(H:H,"Novo")</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>6</v>
@@ -1415,102 +1308,102 @@
         <v>7</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="H5" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="36" t="s">
+      <c r="J5" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="37">
+      <c r="K5" s="36">
         <f>COUNTIF(H:H,"Passou")</f>
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="19" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="H6" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="J6" s="36" t="s">
+      <c r="J6" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="37">
+      <c r="K6" s="36">
         <f>COUNTIF(H:H,"Falhou")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>8</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="19" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="H7" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="J7" s="38" t="s">
+      <c r="J7" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="K7" s="39">
+      <c r="K7" s="38">
         <f>COUNTIF(H:H,"Bloqueado")</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="17" customFormat="1" ht="13" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="H8" s="19" t="s">
         <v>3</v>
@@ -1520,22 +1413,22 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="H9" s="19" t="s">
         <v>3</v>
@@ -1543,22 +1436,22 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="H10" s="19" t="s">
         <v>3</v>
@@ -1566,22 +1459,22 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="G11" s="19" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="H11" s="19" t="s">
         <v>3</v>
@@ -1589,22 +1482,22 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C12" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="D12" s="16" t="s">
-        <v>96</v>
-      </c>
       <c r="E12" s="11" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="G12" s="19" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="H12" s="19" t="s">
         <v>3</v>
@@ -1612,22 +1505,22 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="G13" s="19" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="H13" s="19" t="s">
         <v>3</v>
@@ -1635,22 +1528,22 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="G14" s="19" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="H14" s="19" t="s">
         <v>3</v>
@@ -1658,25 +1551,25 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="H15" s="19" t="s">
         <v>3</v>
@@ -1684,22 +1577,22 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="H16" s="19" t="s">
         <v>3</v>
@@ -1707,22 +1600,22 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="G17" s="19" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="H17" s="19" t="s">
         <v>3</v>
@@ -1730,22 +1623,22 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="G18" s="19" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="H18" s="19" t="s">
         <v>3</v>
@@ -1753,22 +1646,22 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="G19" s="19" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="H19" s="19" t="s">
         <v>3</v>
@@ -1776,22 +1669,22 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="G20" s="19" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="H20" s="19" t="s">
         <v>3</v>
@@ -1799,74 +1692,206 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B21" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="G21" s="19" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="H21" s="19" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
+      <c r="A22" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="G22" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="H22" s="19" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
+      <c r="A23" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="G23" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="H23" s="19" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G24" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="H24" s="19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="G25" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="H25" s="19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="E26" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12" t="s">
+      <c r="G26" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="H26" s="19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F27" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="D24" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="11" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="12"/>
-      <c r="C25" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="F25" s="11" t="s">
+      <c r="G27" s="11" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F26" s="11" t="s">
-        <v>119</v>
-      </c>
+      <c r="H27" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H28" s="19"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H29" s="19"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H30" s="19"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H31" s="19"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H32" s="19"/>
+    </row>
+    <row r="33" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H33" s="19"/>
+    </row>
+    <row r="34" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H34" s="19"/>
+    </row>
+    <row r="35" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H35" s="19"/>
+    </row>
+    <row r="36" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H36" s="19"/>
+    </row>
+    <row r="37" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H37" s="19"/>
+    </row>
+    <row r="38" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H38" s="19"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:H8" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
@@ -1879,7 +1904,7 @@
           <x14:formula1>
             <xm:f>'Caixa Seleção'!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>H3:H23</xm:sqref>
+          <xm:sqref>H3:H21</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1889,144 +1914,111 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99EBE6F-2659-440F-8383-BA8990071465}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="B2:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7265625" style="43" customWidth="1"/>
-    <col min="2" max="3" width="58.453125" style="43" customWidth="1"/>
-    <col min="4" max="16384" width="8.7265625" style="43"/>
+    <col min="1" max="1" width="2.6328125" style="40" customWidth="1"/>
+    <col min="2" max="2" width="24.36328125" style="40" customWidth="1"/>
+    <col min="3" max="3" width="80.7265625" style="40" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.7265625" style="40"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.25">
-      <c r="A1" s="42"/>
-      <c r="B1" s="41" t="s">
-        <v>72</v>
-      </c>
-      <c r="C1" s="41" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="13" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" s="47">
+    <row r="2" spans="2:3" ht="13" x14ac:dyDescent="0.25">
+      <c r="B2" s="52"/>
+      <c r="C2" s="53" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="13" x14ac:dyDescent="0.25">
+      <c r="B3" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="43">
         <v>1</v>
       </c>
-      <c r="C2" s="47">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="13" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" s="50" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="25" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
+    </row>
+    <row r="4" spans="2:3" ht="13" x14ac:dyDescent="0.25">
+      <c r="B4" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="54" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="13" x14ac:dyDescent="0.25">
+      <c r="B5" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="27" t="s">
+      <c r="C5" s="26" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="13" x14ac:dyDescent="0.25">
+      <c r="B6" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="25">
+        <v>45459</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="50" x14ac:dyDescent="0.25">
+      <c r="B7" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="13" x14ac:dyDescent="0.25">
+      <c r="B8" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="13" x14ac:dyDescent="0.25">
+      <c r="B9" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="13" x14ac:dyDescent="0.25">
+      <c r="B10" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="13" x14ac:dyDescent="0.25">
+      <c r="B11" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="13" x14ac:dyDescent="0.25">
+      <c r="B12" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="42" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="13" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="26">
-        <v>45422</v>
-      </c>
-      <c r="C5" s="20">
-        <v>45422</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="50" x14ac:dyDescent="0.25">
-      <c r="A6" s="46" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="13" x14ac:dyDescent="0.25">
-      <c r="A7" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="13" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="13" x14ac:dyDescent="0.25">
-      <c r="A9" s="45" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="13" x14ac:dyDescent="0.25">
-      <c r="A10" s="45" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="13" x14ac:dyDescent="0.25">
-      <c r="A11" s="45" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="192" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" s="28"/>
-      <c r="C12" s="21"/>
+      <c r="C13" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -2042,52 +2034,52 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="50.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" style="23" customWidth="1"/>
-    <col min="2" max="2" width="11.81640625" style="23" customWidth="1"/>
-    <col min="3" max="3" width="36.90625" style="23" customWidth="1"/>
-    <col min="4" max="4" width="10" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.7265625" style="23" customWidth="1"/>
-    <col min="6" max="6" width="32.26953125" style="23" customWidth="1"/>
-    <col min="7" max="7" width="33.6328125" style="23" customWidth="1"/>
-    <col min="8" max="8" width="15.453125" style="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="14.6328125" style="23" customWidth="1"/>
-    <col min="11" max="11" width="25.6328125" style="23" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.6328125" style="23"/>
-    <col min="13" max="14" width="14.54296875" style="23" customWidth="1"/>
-    <col min="15" max="15" width="2.36328125" style="23" customWidth="1"/>
-    <col min="16" max="17" width="14.54296875" style="23" customWidth="1"/>
-    <col min="18" max="16384" width="12.6328125" style="23"/>
+    <col min="1" max="1" width="11" style="22" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" style="22" customWidth="1"/>
+    <col min="3" max="3" width="36.90625" style="22" customWidth="1"/>
+    <col min="4" max="4" width="10" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.7265625" style="22" customWidth="1"/>
+    <col min="6" max="6" width="32.26953125" style="22" customWidth="1"/>
+    <col min="7" max="7" width="33.6328125" style="22" customWidth="1"/>
+    <col min="8" max="8" width="15.453125" style="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="14.6328125" style="22" customWidth="1"/>
+    <col min="11" max="11" width="25.6328125" style="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.6328125" style="22"/>
+    <col min="13" max="14" width="14.54296875" style="22" customWidth="1"/>
+    <col min="15" max="15" width="2.36328125" style="22" customWidth="1"/>
+    <col min="16" max="17" width="14.54296875" style="22" customWidth="1"/>
+    <col min="18" max="16384" width="12.6328125" style="22"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="13" x14ac:dyDescent="0.25">
-      <c r="A1" s="48"/>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="49" t="s">
+      <c r="A1" s="44"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
     </row>
     <row r="2" spans="1:17" ht="26" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>41</v>
@@ -2099,7 +2091,7 @@
         <v>11</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>12</v>
@@ -2111,147 +2103,125 @@
         <v>14</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="50.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29">
+      <c r="A3" s="28">
         <v>1</v>
       </c>
-      <c r="B3" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="25">
-        <v>45422</v>
-      </c>
-      <c r="E3" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="F3" s="21" t="s">
+      <c r="B3" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" s="24">
+        <v>45459</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="G3" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="H3" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="I3" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="J3" s="22" t="s">
+      <c r="M3" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="N3" s="30">
+        <f>SUM(N4:N6)</f>
+        <v>1</v>
+      </c>
+      <c r="P3" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q3" s="30">
+        <f>SUM(Q4:Q6)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="50.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="47"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="51"/>
+      <c r="M4" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" s="39">
+        <f>COUNTIF(I:I,"Alto")</f>
+        <v>1</v>
+      </c>
+      <c r="P4" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="M3" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="N3" s="31">
-        <f>SUM(N4:N6)</f>
-        <v>2</v>
-      </c>
-      <c r="P3" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q3" s="31">
-        <f>SUM(Q4:Q6)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="50.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29">
-        <v>2</v>
-      </c>
-      <c r="B4" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="25">
-        <v>45422</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="G4" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="H4" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="J4" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="M4" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="N4" s="40">
-        <f>COUNTIF(I:I,"Alto")</f>
+      <c r="Q4" s="39">
+        <f>COUNTIF(J:J,"Funcional")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="50.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M5" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" s="39">
+        <f>COUNTIF(I:I,"Médio")</f>
         <v>0</v>
       </c>
-      <c r="P4" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q4" s="40">
-        <f>COUNTIF(J:J,"Funcional")</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="50.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M5" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="N5" s="40">
-        <f>COUNTIF(I:I,"Médio")</f>
-        <v>2</v>
-      </c>
-      <c r="P5" s="40" t="s">
+      <c r="P5" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="Q5" s="40">
+      <c r="Q5" s="39">
         <f>COUNTIF(J:J,"UI/UX")</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="50.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M6" s="40" t="s">
+      <c r="M6" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="N6" s="40">
+      <c r="N6" s="39">
         <f>COUNTIF(I:I,"Baixo")</f>
         <v>0</v>
       </c>
-      <c r="P6" s="40" t="s">
+      <c r="P6" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="Q6" s="40">
+      <c r="Q6" s="39">
         <f>COUNTIF(J:J,"Performance")</f>
         <v>0</v>
       </c>
@@ -2268,32 +2238,29 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9D98E55-3BE0-457D-BCDD-29C0B9CAC6F3}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6328125" style="24" customWidth="1"/>
-    <col min="2" max="2" width="67.36328125" customWidth="1"/>
+    <col min="1" max="1" width="13.6328125" style="23" customWidth="1"/>
+    <col min="2" max="2" width="68.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="29.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="206.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24">
+      <c r="A2" s="23">
         <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="207.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="24">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -2322,11 +2289,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
     </row>
     <row r="2" spans="1:5" ht="5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
@@ -2352,7 +2319,7 @@
       </c>
       <c r="B4" s="8">
         <f>SUM(B5:B7)</f>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C4" s="8">
         <f>SUM(C5:C7)</f>
@@ -2367,7 +2334,7 @@
       </c>
       <c r="B5" s="8">
         <f>COUNTIF(TC!H:H,"Passou")</f>
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C5" s="8">
         <v>0</v>
@@ -2381,7 +2348,7 @@
       </c>
       <c r="B6" s="8">
         <f>COUNTIF(TC!H:H,"Falhou")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="8">
         <v>0</v>
@@ -2429,7 +2396,7 @@
       </c>
       <c r="B10" s="8">
         <f>SUM(B11:B13)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" s="8">
         <f>SUM(C11:C13)</f>
@@ -2444,7 +2411,7 @@
       </c>
       <c r="B11" s="8">
         <f>COUNTIF('Bug Report_Resume'!I:I,"Alto")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="8">
         <v>0</v>
@@ -2458,7 +2425,7 @@
       </c>
       <c r="B12" s="8">
         <f>COUNTIF('Bug Report_Resume'!I:I,"Médio")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C12" s="8">
         <v>0</v>
@@ -2506,7 +2473,7 @@
       </c>
       <c r="B16" s="8">
         <f>SUM(B17:B19)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" s="8">
         <f>SUM(C17:C19)</f>
@@ -2521,7 +2488,7 @@
       </c>
       <c r="B17" s="8">
         <f>COUNTIF('Bug Report_Resume'!J:J,"Funcional")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" s="8">
         <v>0</v>

</xml_diff>